<commit_message>
Add scripts for analyzing slot order and vgroup differences
Added analyze_question_vs_statement.py for analyzing structural differences between questions and statements, and analyze_vgroup_differences.py for comparing absolute slot order patterns across V_group_keys. Also updated the slot order Excel data file.
</commit_message>
<xml_diff>
--- a/training/data/絶対順序考察.xlsx
+++ b/training/data/絶対順序考察.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5B8653-0A32-4725-B66D-504A73267B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5DD71-DDC6-47CC-B59F-1157D6289457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3620" yWindow="3390" windowWidth="32930" windowHeight="17090" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>you</t>
     <phoneticPr fontId="1"/>
@@ -161,6 +161,10 @@
   </si>
   <si>
     <t>wh-word</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gave</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -530,9 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F35997-3EF2-4BE6-981D-19688D794996}">
   <dimension ref="E7:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -668,69 +670,69 @@
     </row>
     <row r="13" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5</v>
-      </c>
-      <c r="L15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" t="s">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add scripts and data for absolute order test cases
Added scripts for analyzing and reorganizing test data, and introduced new absolute order test cases for the 'tell' verb group. Updated data files to include these new cases and removed an obsolete decomposition results file.
</commit_message>
<xml_diff>
--- a/training/data/絶対順序考察.xlsx
+++ b/training/data/絶対順序考察.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5DD71-DDC6-47CC-B59F-1157D6289457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0160C57B-A3E5-4059-85AD-5B99FD46BF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="3390" windowWidth="32930" windowHeight="17090" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
+    <workbookView xWindow="2180" yWindow="2180" windowWidth="35380" windowHeight="18390" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>you</t>
     <phoneticPr fontId="1"/>
@@ -165,6 +165,22 @@
   </si>
   <si>
     <t>gave</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>O1_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>O2_4</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -532,9 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F35997-3EF2-4BE6-981D-19688D794996}">
-  <dimension ref="E7:O16"/>
+  <dimension ref="E7:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -736,6 +754,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add AbsoluteOrderManager and test data for absolute order
Added AbsoluteOrderManager class for dynamic slot ordering in training/data/absolute_order_manager.py. Introduced new test data with absolute order annotations in training/data/final_54_test_data_with_absolute_order_fixed.json. Added fix_case_83.py for correcting slot assignment in case 83. Updated Excel data file.
</commit_message>
<xml_diff>
--- a/training/data/絶対順序考察.xlsx
+++ b/training/data/絶対順序考察.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0160C57B-A3E5-4059-85AD-5B99FD46BF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C431FA-F404-4B37-AFA0-EDBCF6BD08DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="2180" windowWidth="35380" windowHeight="18390" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
+    <workbookView xWindow="2400" yWindow="2620" windowWidth="35380" windowHeight="18390" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,10 +140,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>M3-8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>at the store</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -156,10 +152,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>M2-1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>wh-word</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -181,6 +173,14 @@
   </si>
   <si>
     <t>O2_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M2-8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M1-1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -551,7 +551,7 @@
   <dimension ref="E7:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>20</v>
@@ -582,10 +582,10 @@
         <v>19</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="5:15" x14ac:dyDescent="0.55000000000000004">
@@ -608,10 +608,10 @@
         <v>5</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="5:15" x14ac:dyDescent="0.55000000000000004">
@@ -634,7 +634,7 @@
         <v>21</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="5:15" x14ac:dyDescent="0.55000000000000004">
@@ -657,7 +657,7 @@
         <v>22</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="5:15" x14ac:dyDescent="0.55000000000000004">
@@ -683,18 +683,18 @@
         <v>23</v>
       </c>
       <c r="O11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
         <v>9</v>
@@ -705,13 +705,13 @@
     </row>
     <row r="14" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
         <v>7</v>
@@ -722,13 +722,13 @@
     </row>
     <row r="15" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H15" t="s">
         <v>5</v>
@@ -739,13 +739,13 @@
     </row>
     <row r="16" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -756,16 +756,16 @@
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
         <v>33</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>34</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add eat group analysis scripts and update order logic
Added multiple scripts for analyzing, listing, and mapping elements in the 'eat' group, including scripts for element order, unique elements, and position-based analysis. Updated absolute_order_manager_group_fixed.py to improve element list creation based on sentence word order, with enhanced handling for avoiding element collisions. Also added a script for reading Excel data and updated the related Excel file.
</commit_message>
<xml_diff>
--- a/training/data/絶対順序考察.xlsx
+++ b/training/data/絶対順序考察.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C431FA-F404-4B37-AFA0-EDBCF6BD08DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD635B11-E7E8-4164-962C-DF71CA20AB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="2620" windowWidth="35380" windowHeight="18390" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
+    <workbookView xWindow="2400" yWindow="2620" windowWidth="30560" windowHeight="15620" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>you</t>
     <phoneticPr fontId="1"/>
@@ -180,15 +180,56 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>M1-1</t>
-    <phoneticPr fontId="1"/>
+    <t>M2-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>②</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>③</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>④</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑥</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑦</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⓼</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①What will you eat there?</t>
+  </si>
+  <si>
+    <t>②Will he eat sushi at the park?</t>
+  </si>
+  <si>
+    <t>③How will you eat those stuff?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,13 +245,67 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,12 +322,63 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,40 +694,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F35997-3EF2-4BE6-981D-19688D794996}">
-  <dimension ref="E7:O17"/>
+  <dimension ref="E5:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
+    <row r="5" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="7" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="17" t="s">
         <v>35</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -592,22 +774,24 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M8" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O8" t="s">
@@ -618,22 +802,24 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="H9" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -641,22 +827,24 @@
       <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="H10" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -664,108 +852,165 @@
       <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="M11" s="16"/>
       <c r="O11" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" t="s">
         <v>30</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="5:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" t="s">
         <v>30</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="F17" t="s">
+      <c r="J16" s="10"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="8" t="s">
         <v>34</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="21" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="T21" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="T22" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="T23" s="18" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve adverb position analysis and slot assignment
Enhanced the logic in adverb_position_analyzer.py to more accurately distinguish and merge pre-verb adverb groups (M1, M2), added relative ordering constraints based on sentence context, and improved slot assignment for adverb positions. Updated action_group_fixed_results.json to reflect new slot orderings. Also updated the associated Excel data file.
</commit_message>
<xml_diff>
--- a/training/data/絶対順序考察.xlsx
+++ b/training/data/絶対順序考察.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD635B11-E7E8-4164-962C-DF71CA20AB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62506A57-637A-4B9D-B6B8-168D563D9428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="2620" windowWidth="30560" windowHeight="15620" xr2:uid="{1C274BEB-6454-4DFC-AE89-910D929BA47B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
   <si>
     <t>you</t>
     <phoneticPr fontId="1"/>
@@ -223,6 +223,110 @@
   </si>
   <si>
     <t>③How will you eat those stuff?</t>
+  </si>
+  <si>
+    <t>she</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>beautifully</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>we</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>breakfast</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>always</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>together</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>the cat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>quietly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on the mat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reads</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>books</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>carefully</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>they</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>run</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fast</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>works</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>actually</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>very hard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>every morning</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>he</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jogs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>slowly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>in the park</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -252,7 +356,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +411,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -322,7 +432,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -378,6 +488,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F35997-3EF2-4BE6-981D-19688D794996}">
-  <dimension ref="E5:T23"/>
+  <dimension ref="E5:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1013,8 +1129,235 @@
         <v>47</v>
       </c>
     </row>
+    <row r="24" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>6</v>
+      </c>
+      <c r="L24" s="1">
+        <v>7</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2</v>
+      </c>
+      <c r="P24" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>4</v>
+      </c>
+      <c r="R24" s="1">
+        <v>5</v>
+      </c>
+      <c r="S24" s="1">
+        <v>6</v>
+      </c>
+      <c r="T24" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" t="s">
+        <v>50</v>
+      </c>
+      <c r="O25" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>49</v>
+      </c>
+      <c r="S25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" t="s">
+        <v>51</v>
+      </c>
+      <c r="P26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>52</v>
+      </c>
+      <c r="R26" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" t="s">
+        <v>59</v>
+      </c>
+      <c r="O27" t="s">
+        <v>56</v>
+      </c>
+      <c r="P27" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>57</v>
+      </c>
+      <c r="S27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" t="s">
+        <v>48</v>
+      </c>
+      <c r="P28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>60</v>
+      </c>
+      <c r="R28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" t="s">
+        <v>65</v>
+      </c>
+      <c r="O29" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>64</v>
+      </c>
+      <c r="S29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+      <c r="N30" t="s">
+        <v>67</v>
+      </c>
+      <c r="O30" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>66</v>
+      </c>
+      <c r="S30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="6:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" t="s">
+        <v>73</v>
+      </c>
+      <c r="N31" t="s">
+        <v>69</v>
+      </c>
+      <c r="O31" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>71</v>
+      </c>
+      <c r="S31" t="s">
+        <v>72</v>
+      </c>
+      <c r="T31" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>